<commit_message>
Modif cas d" utilisation + ajout table commande
</commit_message>
<xml_diff>
--- a/fil_rouge/conception/meurice/dictionnaire_donnees.xlsx
+++ b/fil_rouge/conception/meurice/dictionnaire_donnees.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeremy\Desktop\afpa_cda\fil_rouge\conception\meurice\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeremy\Desktop\afpa_cda\CDA_20116-1\fil_rouge\conception\meurice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E21DC5B-8372-4694-949E-BA04E7A64678}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE36F3E4-2D0C-44A3-951C-8E0A6185CFFD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14820" windowHeight="7980" xr2:uid="{AE07E72C-A8ED-4B2A-8334-FB962C1CCAC3}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="110">
   <si>
     <t>Dictionnaire de données - Fil rouge</t>
   </si>
@@ -298,6 +298,63 @@
   </si>
   <si>
     <t>Date</t>
+  </si>
+  <si>
+    <t>OrderDetail</t>
+  </si>
+  <si>
+    <t>Numéro de commandes</t>
+  </si>
+  <si>
+    <t>order_id</t>
+  </si>
+  <si>
+    <t>Date de la commande</t>
+  </si>
+  <si>
+    <t>order_date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nombre de produit commandé </t>
+  </si>
+  <si>
+    <t>product_amount</t>
+  </si>
+  <si>
+    <t>Sous total HT par produit</t>
+  </si>
+  <si>
+    <t>product_sub_total</t>
+  </si>
+  <si>
+    <t>Total HT</t>
+  </si>
+  <si>
+    <t>total_ht</t>
+  </si>
+  <si>
+    <t>Total TTC</t>
+  </si>
+  <si>
+    <t>total_ttc</t>
+  </si>
+  <si>
+    <t>Total des taxes</t>
+  </si>
+  <si>
+    <t>total_tva</t>
+  </si>
+  <si>
+    <t>product_amount * pro_price</t>
+  </si>
+  <si>
+    <t>Sum(product_sub_total)</t>
+  </si>
+  <si>
+    <t>total_ht * tva</t>
+  </si>
+  <si>
+    <t>total_ht * (1+tva)</t>
   </si>
 </sst>
 </file>
@@ -676,8 +733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F209FD6C-FEF6-40FC-969E-2EDADDD0E236}">
   <dimension ref="B1:V104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="R48" sqref="R48"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="N70" sqref="N70:Q70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1922,7 +1979,9 @@
       <c r="Q61" s="2"/>
     </row>
     <row r="62" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B62" s="2"/>
+      <c r="B62" s="3" t="s">
+        <v>91</v>
+      </c>
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
       <c r="E62" s="2"/>
@@ -1940,33 +1999,47 @@
       <c r="Q62" s="2"/>
     </row>
     <row r="63" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B63" s="2"/>
+      <c r="B63" s="2" t="s">
+        <v>92</v>
+      </c>
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
       <c r="E63" s="2"/>
-      <c r="F63" s="2"/>
+      <c r="F63" s="2" t="s">
+        <v>93</v>
+      </c>
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
       <c r="I63" s="2"/>
-      <c r="J63" s="2"/>
+      <c r="J63" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="K63" s="2"/>
       <c r="L63" s="2"/>
       <c r="M63" s="2"/>
-      <c r="N63" s="2"/>
+      <c r="N63" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="O63" s="2"/>
       <c r="P63" s="2"/>
       <c r="Q63" s="2"/>
     </row>
     <row r="64" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B64" s="2"/>
+      <c r="B64" s="2" t="s">
+        <v>94</v>
+      </c>
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
       <c r="E64" s="2"/>
-      <c r="F64" s="2"/>
+      <c r="F64" s="2" t="s">
+        <v>95</v>
+      </c>
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
       <c r="I64" s="2"/>
-      <c r="J64" s="2"/>
+      <c r="J64" s="2" t="s">
+        <v>90</v>
+      </c>
       <c r="K64" s="2"/>
       <c r="L64" s="2"/>
       <c r="M64" s="2"/>
@@ -1976,15 +2049,21 @@
       <c r="Q64" s="2"/>
     </row>
     <row r="65" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B65" s="2"/>
+      <c r="B65" s="2" t="s">
+        <v>96</v>
+      </c>
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
       <c r="E65" s="2"/>
-      <c r="F65" s="2"/>
+      <c r="F65" s="2" t="s">
+        <v>97</v>
+      </c>
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
       <c r="I65" s="2"/>
-      <c r="J65" s="2"/>
+      <c r="J65" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="K65" s="2"/>
       <c r="L65" s="2"/>
       <c r="M65" s="2"/>
@@ -1994,73 +2073,105 @@
       <c r="Q65" s="2"/>
     </row>
     <row r="66" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B66" s="2"/>
+      <c r="B66" s="2" t="s">
+        <v>98</v>
+      </c>
       <c r="C66" s="2"/>
       <c r="D66" s="2"/>
       <c r="E66" s="2"/>
-      <c r="F66" s="2"/>
+      <c r="F66" s="2" t="s">
+        <v>99</v>
+      </c>
       <c r="G66" s="2"/>
       <c r="H66" s="2"/>
       <c r="I66" s="2"/>
-      <c r="J66" s="2"/>
+      <c r="J66" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="K66" s="2"/>
       <c r="L66" s="2"/>
       <c r="M66" s="2"/>
-      <c r="N66" s="2"/>
+      <c r="N66" s="2" t="s">
+        <v>106</v>
+      </c>
       <c r="O66" s="2"/>
       <c r="P66" s="2"/>
       <c r="Q66" s="2"/>
     </row>
     <row r="67" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B67" s="2"/>
+      <c r="B67" s="2" t="s">
+        <v>100</v>
+      </c>
       <c r="C67" s="2"/>
       <c r="D67" s="2"/>
       <c r="E67" s="2"/>
-      <c r="F67" s="2"/>
+      <c r="F67" s="2" t="s">
+        <v>101</v>
+      </c>
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
       <c r="I67" s="2"/>
-      <c r="J67" s="2"/>
+      <c r="J67" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="K67" s="2"/>
       <c r="L67" s="2"/>
       <c r="M67" s="2"/>
-      <c r="N67" s="2"/>
+      <c r="N67" s="2" t="s">
+        <v>107</v>
+      </c>
       <c r="O67" s="2"/>
       <c r="P67" s="2"/>
       <c r="Q67" s="2"/>
     </row>
     <row r="68" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B68" s="2"/>
+      <c r="B68" s="2" t="s">
+        <v>102</v>
+      </c>
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
       <c r="E68" s="2"/>
-      <c r="F68" s="2"/>
+      <c r="F68" s="2" t="s">
+        <v>103</v>
+      </c>
       <c r="G68" s="2"/>
       <c r="H68" s="2"/>
       <c r="I68" s="2"/>
-      <c r="J68" s="2"/>
+      <c r="J68" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="K68" s="2"/>
       <c r="L68" s="2"/>
       <c r="M68" s="2"/>
-      <c r="N68" s="2"/>
+      <c r="N68" s="2" t="s">
+        <v>109</v>
+      </c>
       <c r="O68" s="2"/>
       <c r="P68" s="2"/>
       <c r="Q68" s="2"/>
     </row>
     <row r="69" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B69" s="2"/>
+      <c r="B69" s="2" t="s">
+        <v>104</v>
+      </c>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
       <c r="E69" s="2"/>
-      <c r="F69" s="2"/>
+      <c r="F69" s="2" t="s">
+        <v>105</v>
+      </c>
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
       <c r="I69" s="2"/>
-      <c r="J69" s="2"/>
+      <c r="J69" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="K69" s="2"/>
       <c r="L69" s="2"/>
       <c r="M69" s="2"/>
-      <c r="N69" s="2"/>
+      <c r="N69" s="2" t="s">
+        <v>108</v>
+      </c>
       <c r="O69" s="2"/>
       <c r="P69" s="2"/>
       <c r="Q69" s="2"/>
@@ -2696,16 +2807,310 @@
       <c r="Q104" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="342">
-    <mergeCell ref="F48:I48"/>
-    <mergeCell ref="J48:M48"/>
-    <mergeCell ref="N48:Q48"/>
-    <mergeCell ref="B49:E49"/>
-    <mergeCell ref="F49:I49"/>
-    <mergeCell ref="J49:M49"/>
-    <mergeCell ref="N49:Q49"/>
-    <mergeCell ref="B54:Q54"/>
-    <mergeCell ref="B55:Q55"/>
+  <mergeCells count="336">
+    <mergeCell ref="N39:Q39"/>
+    <mergeCell ref="B10:Q10"/>
+    <mergeCell ref="N35:Q35"/>
+    <mergeCell ref="N36:Q36"/>
+    <mergeCell ref="N27:Q27"/>
+    <mergeCell ref="N30:Q30"/>
+    <mergeCell ref="N31:Q31"/>
+    <mergeCell ref="N32:Q32"/>
+    <mergeCell ref="N22:Q22"/>
+    <mergeCell ref="N23:Q23"/>
+    <mergeCell ref="N24:Q24"/>
+    <mergeCell ref="N25:Q25"/>
+    <mergeCell ref="N26:Q26"/>
+    <mergeCell ref="J39:M39"/>
+    <mergeCell ref="N11:Q11"/>
+    <mergeCell ref="N12:Q12"/>
+    <mergeCell ref="N13:Q13"/>
+    <mergeCell ref="J35:M35"/>
+    <mergeCell ref="J22:M22"/>
+    <mergeCell ref="J23:M23"/>
+    <mergeCell ref="J24:M24"/>
+    <mergeCell ref="J25:M25"/>
+    <mergeCell ref="J26:M26"/>
+    <mergeCell ref="J14:M14"/>
+    <mergeCell ref="J15:M15"/>
+    <mergeCell ref="J16:M16"/>
+    <mergeCell ref="J21:M21"/>
+    <mergeCell ref="J18:M18"/>
+    <mergeCell ref="B39:E39"/>
+    <mergeCell ref="F12:I12"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="F21:I21"/>
+    <mergeCell ref="F18:I18"/>
+    <mergeCell ref="B35:E35"/>
+    <mergeCell ref="B36:E36"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="F35:I35"/>
+    <mergeCell ref="F36:I36"/>
+    <mergeCell ref="F39:I39"/>
+    <mergeCell ref="F30:I30"/>
+    <mergeCell ref="F31:I31"/>
+    <mergeCell ref="F32:I32"/>
+    <mergeCell ref="B34:Q34"/>
+    <mergeCell ref="B33:Q33"/>
+    <mergeCell ref="B37:Q37"/>
+    <mergeCell ref="B38:Q38"/>
+    <mergeCell ref="J36:M36"/>
+    <mergeCell ref="J27:M27"/>
+    <mergeCell ref="J30:M30"/>
+    <mergeCell ref="B30:E30"/>
+    <mergeCell ref="B31:E31"/>
+    <mergeCell ref="B32:E32"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="B28:Q28"/>
+    <mergeCell ref="B29:Q29"/>
+    <mergeCell ref="F22:I22"/>
+    <mergeCell ref="F23:I23"/>
+    <mergeCell ref="F24:I24"/>
+    <mergeCell ref="F25:I25"/>
+    <mergeCell ref="F26:I26"/>
+    <mergeCell ref="F27:I27"/>
+    <mergeCell ref="J31:M31"/>
+    <mergeCell ref="J32:M32"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="B21:E21"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="I1:N6"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="F11:I11"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="J11:M11"/>
+    <mergeCell ref="J12:M12"/>
+    <mergeCell ref="J13:M13"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="J17:M17"/>
+    <mergeCell ref="N17:Q17"/>
+    <mergeCell ref="B19:Q19"/>
+    <mergeCell ref="B20:Q20"/>
+    <mergeCell ref="N14:Q14"/>
+    <mergeCell ref="N15:Q15"/>
+    <mergeCell ref="N16:Q16"/>
+    <mergeCell ref="N21:Q21"/>
+    <mergeCell ref="N18:Q18"/>
+    <mergeCell ref="B56:E56"/>
+    <mergeCell ref="B57:E57"/>
+    <mergeCell ref="B58:E58"/>
+    <mergeCell ref="B59:E59"/>
+    <mergeCell ref="B60:E60"/>
+    <mergeCell ref="B40:E40"/>
+    <mergeCell ref="B43:E43"/>
+    <mergeCell ref="B45:E45"/>
+    <mergeCell ref="B50:E50"/>
+    <mergeCell ref="B51:E51"/>
+    <mergeCell ref="B52:E52"/>
+    <mergeCell ref="B53:E53"/>
+    <mergeCell ref="B48:E48"/>
+    <mergeCell ref="B61:Q61"/>
+    <mergeCell ref="B62:Q62"/>
+    <mergeCell ref="B63:E63"/>
+    <mergeCell ref="B64:E64"/>
+    <mergeCell ref="B65:E65"/>
+    <mergeCell ref="B66:E66"/>
+    <mergeCell ref="B67:E67"/>
+    <mergeCell ref="B68:E68"/>
+    <mergeCell ref="B69:E69"/>
+    <mergeCell ref="B70:E70"/>
+    <mergeCell ref="B71:E71"/>
+    <mergeCell ref="B72:E72"/>
+    <mergeCell ref="B73:E73"/>
+    <mergeCell ref="B74:E74"/>
+    <mergeCell ref="B75:E75"/>
+    <mergeCell ref="B76:E76"/>
+    <mergeCell ref="B77:E77"/>
+    <mergeCell ref="B78:E78"/>
+    <mergeCell ref="B79:E79"/>
+    <mergeCell ref="B80:E80"/>
+    <mergeCell ref="B94:E94"/>
+    <mergeCell ref="B95:E95"/>
+    <mergeCell ref="B96:E96"/>
+    <mergeCell ref="B97:E97"/>
+    <mergeCell ref="B98:E98"/>
+    <mergeCell ref="B81:E81"/>
+    <mergeCell ref="B82:E82"/>
+    <mergeCell ref="B83:E83"/>
+    <mergeCell ref="B84:E84"/>
+    <mergeCell ref="B85:E85"/>
+    <mergeCell ref="B86:E86"/>
+    <mergeCell ref="B87:E87"/>
+    <mergeCell ref="B88:E88"/>
+    <mergeCell ref="B89:E89"/>
+    <mergeCell ref="B99:E99"/>
+    <mergeCell ref="B100:E100"/>
+    <mergeCell ref="B101:E101"/>
+    <mergeCell ref="B102:E102"/>
+    <mergeCell ref="B103:E103"/>
+    <mergeCell ref="B104:E104"/>
+    <mergeCell ref="F40:I40"/>
+    <mergeCell ref="F43:I43"/>
+    <mergeCell ref="F45:I45"/>
+    <mergeCell ref="F50:I50"/>
+    <mergeCell ref="F51:I51"/>
+    <mergeCell ref="F52:I52"/>
+    <mergeCell ref="F53:I53"/>
+    <mergeCell ref="F56:I56"/>
+    <mergeCell ref="F57:I57"/>
+    <mergeCell ref="F58:I58"/>
+    <mergeCell ref="F59:I59"/>
+    <mergeCell ref="F60:I60"/>
+    <mergeCell ref="B90:E90"/>
+    <mergeCell ref="B91:E91"/>
+    <mergeCell ref="B92:E92"/>
+    <mergeCell ref="B93:E93"/>
+    <mergeCell ref="F63:I63"/>
+    <mergeCell ref="F64:I64"/>
+    <mergeCell ref="F65:I65"/>
+    <mergeCell ref="F66:I66"/>
+    <mergeCell ref="F67:I67"/>
+    <mergeCell ref="F68:I68"/>
+    <mergeCell ref="F69:I69"/>
+    <mergeCell ref="F70:I70"/>
+    <mergeCell ref="F71:I71"/>
+    <mergeCell ref="F72:I72"/>
+    <mergeCell ref="F73:I73"/>
+    <mergeCell ref="F74:I74"/>
+    <mergeCell ref="F75:I75"/>
+    <mergeCell ref="F76:I76"/>
+    <mergeCell ref="F77:I77"/>
+    <mergeCell ref="F78:I78"/>
+    <mergeCell ref="F79:I79"/>
+    <mergeCell ref="F80:I80"/>
+    <mergeCell ref="F94:I94"/>
+    <mergeCell ref="F95:I95"/>
+    <mergeCell ref="F96:I96"/>
+    <mergeCell ref="F97:I97"/>
+    <mergeCell ref="F98:I98"/>
+    <mergeCell ref="F81:I81"/>
+    <mergeCell ref="F82:I82"/>
+    <mergeCell ref="F83:I83"/>
+    <mergeCell ref="F84:I84"/>
+    <mergeCell ref="F85:I85"/>
+    <mergeCell ref="F86:I86"/>
+    <mergeCell ref="F87:I87"/>
+    <mergeCell ref="F88:I88"/>
+    <mergeCell ref="F89:I89"/>
+    <mergeCell ref="F99:I99"/>
+    <mergeCell ref="F100:I100"/>
+    <mergeCell ref="F101:I101"/>
+    <mergeCell ref="F102:I102"/>
+    <mergeCell ref="F103:I103"/>
+    <mergeCell ref="F104:I104"/>
+    <mergeCell ref="J40:M40"/>
+    <mergeCell ref="J43:M43"/>
+    <mergeCell ref="J45:M45"/>
+    <mergeCell ref="J50:M50"/>
+    <mergeCell ref="J51:M51"/>
+    <mergeCell ref="J52:M52"/>
+    <mergeCell ref="J53:M53"/>
+    <mergeCell ref="J56:M56"/>
+    <mergeCell ref="J57:M57"/>
+    <mergeCell ref="J58:M58"/>
+    <mergeCell ref="J59:M59"/>
+    <mergeCell ref="J60:M60"/>
+    <mergeCell ref="F90:I90"/>
+    <mergeCell ref="F91:I91"/>
+    <mergeCell ref="F92:I92"/>
+    <mergeCell ref="F93:I93"/>
+    <mergeCell ref="J63:M63"/>
+    <mergeCell ref="J64:M64"/>
+    <mergeCell ref="J65:M65"/>
+    <mergeCell ref="J66:M66"/>
+    <mergeCell ref="J67:M67"/>
+    <mergeCell ref="J68:M68"/>
+    <mergeCell ref="J69:M69"/>
+    <mergeCell ref="J70:M70"/>
+    <mergeCell ref="J71:M71"/>
+    <mergeCell ref="J72:M72"/>
+    <mergeCell ref="J73:M73"/>
+    <mergeCell ref="J74:M74"/>
+    <mergeCell ref="J75:M75"/>
+    <mergeCell ref="J76:M76"/>
+    <mergeCell ref="J77:M77"/>
+    <mergeCell ref="J78:M78"/>
+    <mergeCell ref="J79:M79"/>
+    <mergeCell ref="J80:M80"/>
+    <mergeCell ref="J94:M94"/>
+    <mergeCell ref="J95:M95"/>
+    <mergeCell ref="J96:M96"/>
+    <mergeCell ref="J97:M97"/>
+    <mergeCell ref="J98:M98"/>
+    <mergeCell ref="J81:M81"/>
+    <mergeCell ref="J82:M82"/>
+    <mergeCell ref="J83:M83"/>
+    <mergeCell ref="J84:M84"/>
+    <mergeCell ref="J85:M85"/>
+    <mergeCell ref="J86:M86"/>
+    <mergeCell ref="J87:M87"/>
+    <mergeCell ref="J88:M88"/>
+    <mergeCell ref="J89:M89"/>
+    <mergeCell ref="J99:M99"/>
+    <mergeCell ref="J100:M100"/>
+    <mergeCell ref="J101:M101"/>
+    <mergeCell ref="J102:M102"/>
+    <mergeCell ref="J103:M103"/>
+    <mergeCell ref="J104:M104"/>
+    <mergeCell ref="N40:Q40"/>
+    <mergeCell ref="N43:Q43"/>
+    <mergeCell ref="N45:Q45"/>
+    <mergeCell ref="N50:Q50"/>
+    <mergeCell ref="N51:Q51"/>
+    <mergeCell ref="N52:Q52"/>
+    <mergeCell ref="N53:Q53"/>
+    <mergeCell ref="N56:Q56"/>
+    <mergeCell ref="N57:Q57"/>
+    <mergeCell ref="N58:Q58"/>
+    <mergeCell ref="N59:Q59"/>
+    <mergeCell ref="N60:Q60"/>
+    <mergeCell ref="J90:M90"/>
+    <mergeCell ref="J91:M91"/>
+    <mergeCell ref="J92:M92"/>
+    <mergeCell ref="J93:M93"/>
+    <mergeCell ref="N63:Q63"/>
+    <mergeCell ref="N64:Q64"/>
+    <mergeCell ref="N65:Q65"/>
+    <mergeCell ref="N66:Q66"/>
+    <mergeCell ref="N67:Q67"/>
+    <mergeCell ref="N68:Q68"/>
+    <mergeCell ref="N69:Q69"/>
+    <mergeCell ref="N70:Q70"/>
+    <mergeCell ref="N71:Q71"/>
+    <mergeCell ref="N72:Q72"/>
+    <mergeCell ref="N73:Q73"/>
+    <mergeCell ref="N74:Q74"/>
+    <mergeCell ref="N75:Q75"/>
+    <mergeCell ref="N76:Q76"/>
+    <mergeCell ref="N77:Q77"/>
+    <mergeCell ref="N78:Q78"/>
+    <mergeCell ref="N79:Q79"/>
+    <mergeCell ref="N80:Q80"/>
+    <mergeCell ref="N94:Q94"/>
+    <mergeCell ref="N95:Q95"/>
+    <mergeCell ref="N96:Q96"/>
+    <mergeCell ref="N97:Q97"/>
+    <mergeCell ref="N98:Q98"/>
+    <mergeCell ref="N81:Q81"/>
+    <mergeCell ref="N82:Q82"/>
+    <mergeCell ref="N83:Q83"/>
+    <mergeCell ref="N84:Q84"/>
+    <mergeCell ref="N85:Q85"/>
+    <mergeCell ref="N86:Q86"/>
+    <mergeCell ref="N87:Q87"/>
+    <mergeCell ref="N88:Q88"/>
+    <mergeCell ref="N89:Q89"/>
     <mergeCell ref="N99:Q99"/>
     <mergeCell ref="N100:Q100"/>
     <mergeCell ref="N101:Q101"/>
@@ -2730,315 +3135,15 @@
     <mergeCell ref="N91:Q91"/>
     <mergeCell ref="N92:Q92"/>
     <mergeCell ref="N93:Q93"/>
-    <mergeCell ref="N94:Q94"/>
-    <mergeCell ref="N95:Q95"/>
-    <mergeCell ref="N96:Q96"/>
-    <mergeCell ref="N97:Q97"/>
-    <mergeCell ref="N98:Q98"/>
-    <mergeCell ref="N81:Q81"/>
-    <mergeCell ref="N82:Q82"/>
-    <mergeCell ref="N83:Q83"/>
-    <mergeCell ref="N84:Q84"/>
-    <mergeCell ref="N85:Q85"/>
-    <mergeCell ref="N86:Q86"/>
-    <mergeCell ref="N87:Q87"/>
-    <mergeCell ref="N88:Q88"/>
-    <mergeCell ref="N89:Q89"/>
-    <mergeCell ref="N72:Q72"/>
-    <mergeCell ref="N73:Q73"/>
-    <mergeCell ref="N74:Q74"/>
-    <mergeCell ref="N75:Q75"/>
-    <mergeCell ref="N76:Q76"/>
-    <mergeCell ref="N77:Q77"/>
-    <mergeCell ref="N78:Q78"/>
-    <mergeCell ref="N79:Q79"/>
-    <mergeCell ref="N80:Q80"/>
-    <mergeCell ref="N63:Q63"/>
-    <mergeCell ref="N64:Q64"/>
-    <mergeCell ref="N65:Q65"/>
-    <mergeCell ref="N66:Q66"/>
-    <mergeCell ref="N67:Q67"/>
-    <mergeCell ref="N68:Q68"/>
-    <mergeCell ref="N69:Q69"/>
-    <mergeCell ref="N70:Q70"/>
-    <mergeCell ref="N71:Q71"/>
-    <mergeCell ref="J99:M99"/>
-    <mergeCell ref="J100:M100"/>
-    <mergeCell ref="J101:M101"/>
-    <mergeCell ref="J102:M102"/>
-    <mergeCell ref="J103:M103"/>
-    <mergeCell ref="J104:M104"/>
-    <mergeCell ref="N40:Q40"/>
-    <mergeCell ref="N43:Q43"/>
-    <mergeCell ref="N45:Q45"/>
-    <mergeCell ref="N50:Q50"/>
-    <mergeCell ref="N51:Q51"/>
-    <mergeCell ref="N52:Q52"/>
-    <mergeCell ref="N53:Q53"/>
-    <mergeCell ref="N56:Q56"/>
-    <mergeCell ref="N57:Q57"/>
-    <mergeCell ref="N58:Q58"/>
-    <mergeCell ref="N59:Q59"/>
-    <mergeCell ref="N60:Q60"/>
-    <mergeCell ref="N61:Q61"/>
-    <mergeCell ref="N62:Q62"/>
-    <mergeCell ref="J90:M90"/>
-    <mergeCell ref="J91:M91"/>
-    <mergeCell ref="J92:M92"/>
-    <mergeCell ref="J93:M93"/>
-    <mergeCell ref="J94:M94"/>
-    <mergeCell ref="J95:M95"/>
-    <mergeCell ref="J96:M96"/>
-    <mergeCell ref="J97:M97"/>
-    <mergeCell ref="J98:M98"/>
-    <mergeCell ref="J81:M81"/>
-    <mergeCell ref="J82:M82"/>
-    <mergeCell ref="J83:M83"/>
-    <mergeCell ref="J84:M84"/>
-    <mergeCell ref="J85:M85"/>
-    <mergeCell ref="J86:M86"/>
-    <mergeCell ref="J87:M87"/>
-    <mergeCell ref="J88:M88"/>
-    <mergeCell ref="J89:M89"/>
-    <mergeCell ref="J72:M72"/>
-    <mergeCell ref="J73:M73"/>
-    <mergeCell ref="J74:M74"/>
-    <mergeCell ref="J75:M75"/>
-    <mergeCell ref="J76:M76"/>
-    <mergeCell ref="J77:M77"/>
-    <mergeCell ref="J78:M78"/>
-    <mergeCell ref="J79:M79"/>
-    <mergeCell ref="J80:M80"/>
-    <mergeCell ref="J63:M63"/>
-    <mergeCell ref="J64:M64"/>
-    <mergeCell ref="J65:M65"/>
-    <mergeCell ref="J66:M66"/>
-    <mergeCell ref="J67:M67"/>
-    <mergeCell ref="J68:M68"/>
-    <mergeCell ref="J69:M69"/>
-    <mergeCell ref="J70:M70"/>
-    <mergeCell ref="J71:M71"/>
-    <mergeCell ref="F99:I99"/>
-    <mergeCell ref="F100:I100"/>
-    <mergeCell ref="F101:I101"/>
-    <mergeCell ref="F102:I102"/>
-    <mergeCell ref="F103:I103"/>
-    <mergeCell ref="F104:I104"/>
-    <mergeCell ref="J40:M40"/>
-    <mergeCell ref="J43:M43"/>
-    <mergeCell ref="J45:M45"/>
-    <mergeCell ref="J50:M50"/>
-    <mergeCell ref="J51:M51"/>
-    <mergeCell ref="J52:M52"/>
-    <mergeCell ref="J53:M53"/>
-    <mergeCell ref="J56:M56"/>
-    <mergeCell ref="J57:M57"/>
-    <mergeCell ref="J58:M58"/>
-    <mergeCell ref="J59:M59"/>
-    <mergeCell ref="J60:M60"/>
-    <mergeCell ref="J61:M61"/>
-    <mergeCell ref="J62:M62"/>
-    <mergeCell ref="F90:I90"/>
-    <mergeCell ref="F91:I91"/>
-    <mergeCell ref="F92:I92"/>
-    <mergeCell ref="F93:I93"/>
-    <mergeCell ref="F94:I94"/>
-    <mergeCell ref="F95:I95"/>
-    <mergeCell ref="F96:I96"/>
-    <mergeCell ref="F97:I97"/>
-    <mergeCell ref="F98:I98"/>
-    <mergeCell ref="F81:I81"/>
-    <mergeCell ref="F82:I82"/>
-    <mergeCell ref="F83:I83"/>
-    <mergeCell ref="F84:I84"/>
-    <mergeCell ref="F85:I85"/>
-    <mergeCell ref="F86:I86"/>
-    <mergeCell ref="F87:I87"/>
-    <mergeCell ref="F88:I88"/>
-    <mergeCell ref="F89:I89"/>
-    <mergeCell ref="F72:I72"/>
-    <mergeCell ref="F73:I73"/>
-    <mergeCell ref="F74:I74"/>
-    <mergeCell ref="F75:I75"/>
-    <mergeCell ref="F76:I76"/>
-    <mergeCell ref="F77:I77"/>
-    <mergeCell ref="F78:I78"/>
-    <mergeCell ref="F79:I79"/>
-    <mergeCell ref="F80:I80"/>
-    <mergeCell ref="F63:I63"/>
-    <mergeCell ref="F64:I64"/>
-    <mergeCell ref="F65:I65"/>
-    <mergeCell ref="F66:I66"/>
-    <mergeCell ref="F67:I67"/>
-    <mergeCell ref="F68:I68"/>
-    <mergeCell ref="F69:I69"/>
-    <mergeCell ref="F70:I70"/>
-    <mergeCell ref="F71:I71"/>
-    <mergeCell ref="B99:E99"/>
-    <mergeCell ref="B100:E100"/>
-    <mergeCell ref="B101:E101"/>
-    <mergeCell ref="B102:E102"/>
-    <mergeCell ref="B103:E103"/>
-    <mergeCell ref="B104:E104"/>
-    <mergeCell ref="F40:I40"/>
-    <mergeCell ref="F43:I43"/>
-    <mergeCell ref="F45:I45"/>
-    <mergeCell ref="F50:I50"/>
-    <mergeCell ref="F51:I51"/>
-    <mergeCell ref="F52:I52"/>
-    <mergeCell ref="F53:I53"/>
-    <mergeCell ref="F56:I56"/>
-    <mergeCell ref="F57:I57"/>
-    <mergeCell ref="F58:I58"/>
-    <mergeCell ref="F59:I59"/>
-    <mergeCell ref="F60:I60"/>
-    <mergeCell ref="F61:I61"/>
-    <mergeCell ref="F62:I62"/>
-    <mergeCell ref="B90:E90"/>
-    <mergeCell ref="B91:E91"/>
-    <mergeCell ref="B92:E92"/>
-    <mergeCell ref="B93:E93"/>
-    <mergeCell ref="B94:E94"/>
-    <mergeCell ref="B95:E95"/>
-    <mergeCell ref="B96:E96"/>
-    <mergeCell ref="B97:E97"/>
-    <mergeCell ref="B98:E98"/>
-    <mergeCell ref="B81:E81"/>
-    <mergeCell ref="B82:E82"/>
-    <mergeCell ref="B83:E83"/>
-    <mergeCell ref="B84:E84"/>
-    <mergeCell ref="B85:E85"/>
-    <mergeCell ref="B86:E86"/>
-    <mergeCell ref="B87:E87"/>
-    <mergeCell ref="B88:E88"/>
-    <mergeCell ref="B89:E89"/>
-    <mergeCell ref="B72:E72"/>
-    <mergeCell ref="B73:E73"/>
-    <mergeCell ref="B74:E74"/>
-    <mergeCell ref="B75:E75"/>
-    <mergeCell ref="B76:E76"/>
-    <mergeCell ref="B77:E77"/>
-    <mergeCell ref="B78:E78"/>
-    <mergeCell ref="B79:E79"/>
-    <mergeCell ref="B80:E80"/>
-    <mergeCell ref="B63:E63"/>
-    <mergeCell ref="B64:E64"/>
-    <mergeCell ref="B65:E65"/>
-    <mergeCell ref="B66:E66"/>
-    <mergeCell ref="B67:E67"/>
-    <mergeCell ref="B68:E68"/>
-    <mergeCell ref="B69:E69"/>
-    <mergeCell ref="B70:E70"/>
-    <mergeCell ref="B71:E71"/>
-    <mergeCell ref="B56:E56"/>
-    <mergeCell ref="B57:E57"/>
-    <mergeCell ref="B58:E58"/>
-    <mergeCell ref="B59:E59"/>
-    <mergeCell ref="B60:E60"/>
-    <mergeCell ref="B61:E61"/>
-    <mergeCell ref="B62:E62"/>
-    <mergeCell ref="B40:E40"/>
-    <mergeCell ref="B43:E43"/>
-    <mergeCell ref="B45:E45"/>
-    <mergeCell ref="B50:E50"/>
-    <mergeCell ref="B51:E51"/>
-    <mergeCell ref="B52:E52"/>
-    <mergeCell ref="B53:E53"/>
-    <mergeCell ref="B48:E48"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="B16:E16"/>
-    <mergeCell ref="B21:E21"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="I1:N6"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="F11:I11"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="J11:M11"/>
-    <mergeCell ref="J12:M12"/>
-    <mergeCell ref="J13:M13"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="J17:M17"/>
-    <mergeCell ref="N17:Q17"/>
-    <mergeCell ref="B19:Q19"/>
-    <mergeCell ref="B20:Q20"/>
-    <mergeCell ref="B30:E30"/>
-    <mergeCell ref="B31:E31"/>
-    <mergeCell ref="B32:E32"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="B25:E25"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="B28:Q28"/>
-    <mergeCell ref="B29:Q29"/>
-    <mergeCell ref="F22:I22"/>
-    <mergeCell ref="F23:I23"/>
-    <mergeCell ref="F24:I24"/>
-    <mergeCell ref="F25:I25"/>
-    <mergeCell ref="F26:I26"/>
-    <mergeCell ref="F27:I27"/>
-    <mergeCell ref="B39:E39"/>
-    <mergeCell ref="F12:I12"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="F14:I14"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="F16:I16"/>
-    <mergeCell ref="F21:I21"/>
-    <mergeCell ref="F18:I18"/>
-    <mergeCell ref="B35:E35"/>
-    <mergeCell ref="B36:E36"/>
-    <mergeCell ref="B27:E27"/>
-    <mergeCell ref="F35:I35"/>
-    <mergeCell ref="F36:I36"/>
-    <mergeCell ref="F39:I39"/>
-    <mergeCell ref="F30:I30"/>
-    <mergeCell ref="F31:I31"/>
-    <mergeCell ref="F32:I32"/>
-    <mergeCell ref="B34:Q34"/>
-    <mergeCell ref="B33:Q33"/>
-    <mergeCell ref="B37:Q37"/>
-    <mergeCell ref="B38:Q38"/>
-    <mergeCell ref="J36:M36"/>
-    <mergeCell ref="J27:M27"/>
-    <mergeCell ref="J30:M30"/>
-    <mergeCell ref="J31:M31"/>
-    <mergeCell ref="J32:M32"/>
-    <mergeCell ref="N14:Q14"/>
-    <mergeCell ref="N15:Q15"/>
-    <mergeCell ref="N16:Q16"/>
-    <mergeCell ref="N21:Q21"/>
-    <mergeCell ref="N18:Q18"/>
-    <mergeCell ref="J35:M35"/>
-    <mergeCell ref="J22:M22"/>
-    <mergeCell ref="J23:M23"/>
-    <mergeCell ref="J24:M24"/>
-    <mergeCell ref="J25:M25"/>
-    <mergeCell ref="J26:M26"/>
-    <mergeCell ref="J14:M14"/>
-    <mergeCell ref="J15:M15"/>
-    <mergeCell ref="J16:M16"/>
-    <mergeCell ref="J21:M21"/>
-    <mergeCell ref="J18:M18"/>
-    <mergeCell ref="N39:Q39"/>
-    <mergeCell ref="B10:Q10"/>
-    <mergeCell ref="N35:Q35"/>
-    <mergeCell ref="N36:Q36"/>
-    <mergeCell ref="N27:Q27"/>
-    <mergeCell ref="N30:Q30"/>
-    <mergeCell ref="N31:Q31"/>
-    <mergeCell ref="N32:Q32"/>
-    <mergeCell ref="N22:Q22"/>
-    <mergeCell ref="N23:Q23"/>
-    <mergeCell ref="N24:Q24"/>
-    <mergeCell ref="N25:Q25"/>
-    <mergeCell ref="N26:Q26"/>
-    <mergeCell ref="J39:M39"/>
-    <mergeCell ref="N11:Q11"/>
-    <mergeCell ref="N12:Q12"/>
-    <mergeCell ref="N13:Q13"/>
+    <mergeCell ref="F48:I48"/>
+    <mergeCell ref="J48:M48"/>
+    <mergeCell ref="N48:Q48"/>
+    <mergeCell ref="B49:E49"/>
+    <mergeCell ref="F49:I49"/>
+    <mergeCell ref="J49:M49"/>
+    <mergeCell ref="N49:Q49"/>
+    <mergeCell ref="B54:Q54"/>
+    <mergeCell ref="B55:Q55"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>